<commit_message>
refactoring and getting answer options to display in buttons
</commit_message>
<xml_diff>
--- a/classdiagram.xlsx
+++ b/classdiagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garethharris/AndroidStudioProjects/hiragana_katakana/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5F754F-AD79-5C43-BF2E-331A02DCA43E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CB81C4-3417-6842-9F4B-D43EF9841FF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="4060" windowWidth="28800" windowHeight="17540" xr2:uid="{ED955C30-5B55-7C4A-A680-65B318D7E8D7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>hiragana</t>
   </si>
@@ -83,9 +83,6 @@
     <t>answers</t>
   </si>
   <si>
-    <t>QuestionModel</t>
-  </si>
-  <si>
     <t>character</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>Character Model</t>
   </si>
   <si>
-    <t>Question Model</t>
-  </si>
-  <si>
     <t>Character Controller</t>
   </si>
   <si>
@@ -129,6 +123,27 @@
   </si>
   <si>
     <t>nextQuestion()</t>
+  </si>
+  <si>
+    <t>AnswerModel</t>
+  </si>
+  <si>
+    <t>Answer Model</t>
+  </si>
+  <si>
+    <t>userAnswer</t>
+  </si>
+  <si>
+    <t>getCharacters</t>
+  </si>
+  <si>
+    <t>generateQuestions</t>
+  </si>
+  <si>
+    <t>quizController</t>
+  </si>
+  <si>
+    <t>displayAnswer</t>
   </si>
 </sst>
 </file>
@@ -513,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2B308B-5C5E-A544-B8A7-7DAA485E4A30}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J8"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -527,12 +542,12 @@
     <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="J1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -540,7 +555,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -555,12 +570,12 @@
         <v>7</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="J3" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -568,13 +583,13 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -583,7 +598,7 @@
         <v>12</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -591,27 +606,30 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="J5" t="s">
-        <v>25</v>
+      <c r="J5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="J6" t="s">
-        <v>26</v>
+      <c r="J6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -625,24 +643,44 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="F8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="E9" s="3"/>
-      <c r="J9" t="s">
-        <v>29</v>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
answer options update when questioned in answered
</commit_message>
<xml_diff>
--- a/classdiagram.xlsx
+++ b/classdiagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garethharris/AndroidStudioProjects/hiragana_katakana/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CB81C4-3417-6842-9F4B-D43EF9841FF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9255D648-E514-ED47-B974-60D3CCBB0E02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="4060" windowWidth="28800" windowHeight="17540" xr2:uid="{ED955C30-5B55-7C4A-A680-65B318D7E8D7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>hiragana</t>
   </si>
@@ -132,18 +132,6 @@
   </si>
   <si>
     <t>userAnswer</t>
-  </si>
-  <si>
-    <t>getCharacters</t>
-  </si>
-  <si>
-    <t>generateQuestions</t>
-  </si>
-  <si>
-    <t>quizController</t>
-  </si>
-  <si>
-    <t>displayAnswer</t>
   </si>
 </sst>
 </file>
@@ -528,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2B308B-5C5E-A544-B8A7-7DAA485E4A30}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A14" sqref="A14:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -663,26 +651,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>